<commit_message>
deployment rws & bmg
</commit_message>
<xml_diff>
--- a/Traveloka_DataAutomation_Portal_Bemyguest/Data/Config.xlsx
+++ b/Traveloka_DataAutomation_Portal_Bemyguest/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Kalyana\dataautomation_personal\Traveloka_DataAutomation_Portal_Bemyguest\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16C6471A-30F1-41CC-9F78-3A59FC1B37BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26D5AAA0-9EDD-46E4-90B1-ED04409EF844}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="28992" windowHeight="14736" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -191,9 +191,6 @@
     <t>Captcha_RuleId</t>
   </si>
   <si>
-    <t>[Dev] RPA_Moon_UploadBucket</t>
-  </si>
-  <si>
     <t>OrchestratorQueueName</t>
   </si>
   <si>
@@ -203,21 +200,6 @@
     <t>DialogDownloadChrome</t>
   </si>
   <si>
-    <t>[Dev] RPA_Moon_PathMasterFolder</t>
-  </si>
-  <si>
-    <t>[Dev] RPA_Moon_PathMailTemplate</t>
-  </si>
-  <si>
-    <t>[Dev] RPA_Moon_PathSaKey</t>
-  </si>
-  <si>
-    <t>[Dev] RPA_Moon_PathDownloadChrome</t>
-  </si>
-  <si>
-    <t>[Dev] RPA_Moon_DialogDownloadChrome</t>
-  </si>
-  <si>
     <t>SenderName</t>
   </si>
   <si>
@@ -239,7 +221,25 @@
     <t>RPA_Moon_Cred_Gmail</t>
   </si>
   <si>
-    <t>[Dev] RPA_Moon_SheetIdConfig_Experience</t>
+    <t>RPA_Moon_UploadBucket</t>
+  </si>
+  <si>
+    <t>RPA_Moon_PathMasterFolder</t>
+  </si>
+  <si>
+    <t>RPA_Moon_PathMailTemplate</t>
+  </si>
+  <si>
+    <t>RPA_Moon_PathSaKey</t>
+  </si>
+  <si>
+    <t>RPA_Moon_PathDownloadChrome</t>
+  </si>
+  <si>
+    <t>RPA_Moon_DialogDownloadChrome</t>
+  </si>
+  <si>
+    <t>RPA_Moon_SheetIdConfig_Experience</t>
   </si>
 </sst>
 </file>
@@ -666,10 +666,10 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>21</v>
@@ -707,7 +707,7 @@
         <v>44</v>
       </c>
       <c r="B7" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="C7" t="s">
         <v>45</v>
@@ -2877,7 +2877,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1"/>
@@ -2937,7 +2937,7 @@
         <v>42</v>
       </c>
       <c r="B3" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
@@ -2945,7 +2945,7 @@
         <v>46</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
@@ -2953,7 +2953,7 @@
         <v>49</v>
       </c>
       <c r="B5" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
@@ -2961,7 +2961,7 @@
         <v>50</v>
       </c>
       <c r="B6" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
@@ -2969,39 +2969,39 @@
         <v>51</v>
       </c>
       <c r="B7" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="B8" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B9" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B10" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
       <c r="A11" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="B11" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>